<commit_message>
Algorithm changed with seminar groups
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossf\Dropbox\fairnessSeKo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossf\Dropbox\fairnessSeKo\git\gluecksfee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C72F4C6-A8FF-4B98-8676-BBCC8337264B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66139C90-0D23-4328-827F-72A88F653DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39660" yWindow="1230" windowWidth="31050" windowHeight="18630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7050" yWindow="4500" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registrierung" sheetId="1" r:id="rId1"/>
@@ -31,38 +31,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Anna</t>
   </si>
   <si>
-    <t>Yoga</t>
-  </si>
-  <si>
     <t>Plaetze</t>
   </si>
   <si>
-    <t>Python für Anfänger</t>
-  </si>
-  <si>
     <t>Hundeerziehung</t>
   </si>
   <si>
-    <t>Informatik Einführung</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
-    <t>Klimaneutralität</t>
-  </si>
-  <si>
-    <t>Herbstlaubbastelarbeit</t>
-  </si>
-  <si>
-    <t>Moderation von Seminaren</t>
-  </si>
-  <si>
     <t>Ben</t>
   </si>
   <si>
@@ -207,19 +189,46 @@
     <t>Tandemfahren</t>
   </si>
   <si>
-    <t>Reggae tanzen</t>
+    <t>inhaltlich</t>
+  </si>
+  <si>
+    <t>Python für Anfänger A</t>
+  </si>
+  <si>
+    <t>Python für Anfänger B</t>
+  </si>
+  <si>
+    <t>Informatik Einführung A</t>
+  </si>
+  <si>
+    <t>Informatik Einführung B</t>
+  </si>
+  <si>
+    <t>Klimaneutralität A</t>
+  </si>
+  <si>
+    <t>Klimaneutralität B</t>
+  </si>
+  <si>
+    <t>Klimaneutralität C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -243,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -257,6 +266,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -513,20 +528,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:K49" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:K50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Person" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Python für Anfänger" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Yoga" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Python für Anfänger A" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Python für Anfänger B" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tandemfahren" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Hundeerziehung" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Vegan kochen" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Reggae tanzen" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Informatik Einführung" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Klimaneutralität" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Herbstlaubbastelarbeit" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Moderation von Seminaren" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Informatik Einführung A" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Informatik Einführung B" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Klimaneutralität A" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Klimaneutralität B" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Klimaneutralität C" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,115 +891,115 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>4</v>
+      </c>
+      <c r="G2" s="8">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="J2" s="8">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>17</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>15</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>14</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>14</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>14</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H3" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I3" s="2">
         <v>14</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J3" s="2">
         <v>14</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K3" s="2">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -993,22 +1008,22 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
@@ -1016,34 +1031,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -1051,13 +1066,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1066,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -1078,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -1086,7 +1101,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -1095,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -1104,13 +1119,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
@@ -1121,7 +1136,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -1130,22 +1145,22 @@
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -1156,7 +1171,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1165,13 +1180,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -1191,7 +1206,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -1203,16 +1218,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -1226,16 +1241,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1247,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -1261,22 +1276,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
@@ -1285,56 +1300,56 @@
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2">
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1352,13 +1367,13 @@
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2">
         <v>0</v>
@@ -1366,7 +1381,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -1387,13 +1402,13 @@
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -1401,16 +1416,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -1419,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
@@ -1436,57 +1451,57 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="2">
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -1501,27 +1516,27 @@
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -1533,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
@@ -1541,22 +1556,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -1565,10 +1580,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -1576,7 +1591,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -1591,33 +1606,33 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
       </c>
       <c r="H21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2">
         <v>0</v>
       </c>
       <c r="K21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1629,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2">
         <v>1</v>
@@ -1638,15 +1653,15 @@
         <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
@@ -1655,16 +1670,16 @@
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2">
         <v>1</v>
@@ -1673,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
@@ -1681,7 +1696,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -1690,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -1702,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -1716,7 +1731,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
@@ -1725,19 +1740,19 @@
         <v>1</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
       <c r="H25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2">
         <v>0</v>
@@ -1751,13 +1766,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -1772,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -1786,22 +1801,22 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
@@ -1810,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="2">
         <v>0</v>
@@ -1821,7 +1836,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
@@ -1836,48 +1851,48 @@
         <v>1</v>
       </c>
       <c r="F28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
       </c>
       <c r="H28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
         <v>0</v>
       </c>
       <c r="K28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
       </c>
       <c r="F29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
       </c>
       <c r="H29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -1886,24 +1901,24 @@
         <v>0</v>
       </c>
       <c r="K29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -1915,7 +1930,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="2">
         <v>0</v>
@@ -1926,31 +1941,31 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="2">
         <v>0</v>
@@ -1961,16 +1976,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
@@ -1979,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
@@ -1988,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
@@ -1996,22 +2011,22 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>
       </c>
       <c r="F33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
@@ -2023,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
@@ -2031,22 +2046,22 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
@@ -2058,18 +2073,18 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -2078,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -2087,13 +2102,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="2">
         <v>1</v>
@@ -2101,7 +2116,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
@@ -2116,13 +2131,13 @@
         <v>1</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="2">
         <v>0</v>
       </c>
       <c r="H36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -2131,12 +2146,12 @@
         <v>0</v>
       </c>
       <c r="K36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
@@ -2145,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="2">
         <v>1</v>
@@ -2166,27 +2181,27 @@
         <v>0</v>
       </c>
       <c r="K37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="2">
         <v>1</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
@@ -2201,33 +2216,33 @@
         <v>0</v>
       </c>
       <c r="K38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="2">
         <v>0</v>
       </c>
       <c r="D39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
         <v>0</v>
       </c>
       <c r="H39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="2">
         <v>0</v>
@@ -2241,16 +2256,16 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="2">
         <v>0</v>
@@ -2262,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="2">
         <v>0</v>
@@ -2276,7 +2291,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
@@ -2285,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="2">
         <v>0</v>
@@ -2297,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -2306,12 +2321,12 @@
         <v>0</v>
       </c>
       <c r="K41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
@@ -2320,19 +2335,19 @@
         <v>1</v>
       </c>
       <c r="D42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2">
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="2">
         <v>0</v>
@@ -2346,69 +2361,69 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="C43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
       </c>
       <c r="E43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="2">
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
       </c>
       <c r="E44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2">
         <v>0</v>
       </c>
       <c r="H44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
@@ -2416,19 +2431,19 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
@@ -2446,18 +2461,18 @@
         <v>0</v>
       </c>
       <c r="K45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
@@ -2466,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="2">
         <v>0</v>
@@ -2481,12 +2496,12 @@
         <v>0</v>
       </c>
       <c r="K46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
@@ -2501,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="2">
         <v>0</v>
@@ -2521,34 +2536,34 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
       </c>
       <c r="C48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
       </c>
       <c r="F48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
       </c>
       <c r="H48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" s="2">
         <v>0</v>
@@ -2556,36 +2571,71 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B49" s="2">
         <v>1</v>
       </c>
       <c r="C49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
       </c>
       <c r="G49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
       </c>
       <c r="K49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>1</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1</v>
+      </c>
+      <c r="K50" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>